<commit_message>
Upload project plan and update README
</commit_message>
<xml_diff>
--- a/mgmt/project-plan.xlsx
+++ b/mgmt/project-plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2475\Documents\GitHub\building-cicd-pipeline\mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBA1B01-A160-42B0-B028-ED29386649CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5A6F75-1FFF-46C3-B168-5DD379DD62E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,48 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Week</t>
-  </si>
-  <si>
-    <t>2021-KW26</t>
-  </si>
-  <si>
-    <t>2021-KW27</t>
-  </si>
-  <si>
-    <t>2021-KW28</t>
-  </si>
-  <si>
-    <t>2021-KW29</t>
-  </si>
-  <si>
-    <t>2021-KW30</t>
-  </si>
-  <si>
-    <t>2021-KW31</t>
-  </si>
-  <si>
-    <t>2021-KW32</t>
-  </si>
-  <si>
-    <t>2021-KW33</t>
-  </si>
-  <si>
-    <t>2021-KW34</t>
-  </si>
-  <si>
-    <t>2021-KW35</t>
-  </si>
-  <si>
-    <t>2021-KW36</t>
-  </si>
-  <si>
-    <t>2021-KW37</t>
-  </si>
-  <si>
-    <t>QA-Cushion</t>
   </si>
   <si>
     <t>Goals per Component</t>
@@ -79,46 +40,93 @@
     <t>Test continuous delivery</t>
   </si>
   <si>
-    <t>API that returns no data</t>
-  </si>
-  <si>
-    <t>Connects to an API</t>
-  </si>
-  <si>
-    <t>ML API</t>
-  </si>
-  <si>
-    <t>Deploy on Azure</t>
-  </si>
-  <si>
-    <t>Python/Flask</t>
-  </si>
-  <si>
-    <t>Implement build process</t>
-  </si>
-  <si>
-    <t>Logging</t>
-  </si>
-  <si>
     <t>Use of Github Actions</t>
   </si>
   <si>
     <t>Use of Azure Pipelines</t>
   </si>
   <si>
-    <t>Deploy AZ AppService</t>
+    <t>Implement build process on Azure Pipelines</t>
   </si>
   <si>
-    <t>Test Flask ML API</t>
+    <t>2021-CW26</t>
   </si>
   <si>
-    <t>Set up Source Control
-Implement basic build process
-using GitHub Actions
-Test build process locally</t>
+    <t>2021-CW18</t>
   </si>
   <si>
-    <t>Implement build process on Azure Pipelines</t>
+    <t>2021-CW19</t>
+  </si>
+  <si>
+    <t>2021-CW20</t>
+  </si>
+  <si>
+    <t>2021-CW21</t>
+  </si>
+  <si>
+    <t>2021-CW22</t>
+  </si>
+  <si>
+    <t>2021-CW23</t>
+  </si>
+  <si>
+    <t>2021-CW24</t>
+  </si>
+  <si>
+    <t>2021-CW25</t>
+  </si>
+  <si>
+    <t>Deploy WebApp on Azure</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Create project plan</t>
+  </si>
+  <si>
+    <t>Create GitHub repo with scaffolding code</t>
+  </si>
+  <si>
+    <t>Take screenshots and maintain README</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create architectural diagram and maintain README </t>
+  </si>
+  <si>
+    <t>Test build process locally</t>
+  </si>
+  <si>
+    <t>Implement basic build process
+using GitHub Actions</t>
+  </si>
+  <si>
+    <t>Create a trello board</t>
+  </si>
+  <si>
+    <t>Deploy AppService on Azure</t>
+  </si>
+  <si>
+    <t>Test AppService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Add full instructrutions to README on how to run the code</t>
+  </si>
+  <si>
+    <t>Finalize README</t>
+  </si>
+  <si>
+    <t>Record demo video</t>
+  </si>
+  <si>
+    <t>First submit of project</t>
   </si>
 </sst>
 </file>
@@ -128,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -159,13 +167,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -209,7 +210,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -237,14 +238,21 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -465,10 +473,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -481,7 +489,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
@@ -489,10 +497,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -518,15 +526,15 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>30</v>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>24</v>
+      <c r="C3" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="10"/>
@@ -553,11 +561,9 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
+      <c r="A4" s="3"/>
+      <c r="C4" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="10"/>
@@ -583,15 +589,15 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
+      <c r="B5" s="12" t="s">
+        <v>26</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>18</v>
+      <c r="C5" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="10"/>
@@ -618,16 +624,14 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
+      <c r="A6" s="3"/>
+      <c r="B6" s="12" t="s">
+        <v>25</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -651,15 +655,13 @@
     </row>
     <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -683,13 +685,13 @@
     </row>
     <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -711,15 +713,17 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
+    <row r="9" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="12" t="s">
+        <v>28</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -741,17 +745,17 @@
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
     </row>
-    <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
+    <row r="10" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="12" t="s">
+        <v>29</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="10" t="s">
-        <v>28</v>
+      <c r="C10" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -774,16 +778,14 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
+      <c r="A11" s="3"/>
+      <c r="B11" s="12" t="s">
+        <v>8</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="C11" s="12"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -805,15 +807,19 @@
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -837,15 +843,13 @@
     </row>
     <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -869,13 +873,13 @@
     </row>
     <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -898,50 +902,46 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="10" t="s">
-        <v>21</v>
+      <c r="A16" s="3" t="s">
+        <v>9</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>22</v>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -964,16 +964,13 @@
       <c r="Z16" s="4"/>
     </row>
     <row r="17" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="B17" s="12"/>
       <c r="C17" s="10" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -996,14 +993,13 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="11" t="s">
-        <v>26</v>
+      <c r="B18" s="12"/>
+      <c r="C18" s="10" t="s">
+        <v>34</v>
       </c>
-      <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1026,39 +1022,47 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="11" t="s">
-        <v>27</v>
+      <c r="A19" s="7" t="s">
+        <v>1</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
+      <c r="B19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1085,8 +1089,10 @@
     </row>
     <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="10"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1113,7 +1119,6 @@
     </row>
     <row r="22" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1141,7 +1146,6 @@
     </row>
     <row r="23" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -28551,10 +28555,119 @@
       <c r="Y1001" s="4"/>
       <c r="Z1001" s="4"/>
     </row>
+    <row r="1002" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1002" s="6"/>
+      <c r="B1002" s="4"/>
+      <c r="C1002" s="4"/>
+      <c r="D1002" s="4"/>
+      <c r="E1002" s="4"/>
+      <c r="F1002" s="4"/>
+      <c r="G1002" s="4"/>
+      <c r="H1002" s="4"/>
+      <c r="I1002" s="4"/>
+      <c r="J1002" s="4"/>
+      <c r="K1002" s="4"/>
+      <c r="L1002" s="4"/>
+      <c r="M1002" s="4"/>
+      <c r="N1002" s="4"/>
+      <c r="O1002" s="4"/>
+      <c r="P1002" s="4"/>
+      <c r="Q1002" s="4"/>
+      <c r="R1002" s="4"/>
+      <c r="S1002" s="4"/>
+      <c r="T1002" s="4"/>
+      <c r="U1002" s="4"/>
+      <c r="V1002" s="4"/>
+      <c r="W1002" s="4"/>
+      <c r="X1002" s="4"/>
+      <c r="Y1002" s="4"/>
+      <c r="Z1002" s="4"/>
+    </row>
+    <row r="1003" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1003" s="6"/>
+      <c r="B1003" s="4"/>
+      <c r="C1003" s="4"/>
+      <c r="D1003" s="4"/>
+      <c r="E1003" s="4"/>
+      <c r="F1003" s="4"/>
+      <c r="G1003" s="4"/>
+      <c r="H1003" s="4"/>
+      <c r="I1003" s="4"/>
+      <c r="J1003" s="4"/>
+      <c r="K1003" s="4"/>
+      <c r="L1003" s="4"/>
+      <c r="M1003" s="4"/>
+      <c r="N1003" s="4"/>
+      <c r="O1003" s="4"/>
+      <c r="P1003" s="4"/>
+      <c r="Q1003" s="4"/>
+      <c r="R1003" s="4"/>
+      <c r="S1003" s="4"/>
+      <c r="T1003" s="4"/>
+      <c r="U1003" s="4"/>
+      <c r="V1003" s="4"/>
+      <c r="W1003" s="4"/>
+      <c r="X1003" s="4"/>
+      <c r="Y1003" s="4"/>
+      <c r="Z1003" s="4"/>
+    </row>
+    <row r="1004" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1004" s="6"/>
+      <c r="B1004" s="4"/>
+      <c r="C1004" s="4"/>
+      <c r="D1004" s="4"/>
+      <c r="E1004" s="4"/>
+      <c r="F1004" s="4"/>
+      <c r="G1004" s="4"/>
+      <c r="H1004" s="4"/>
+      <c r="I1004" s="4"/>
+      <c r="J1004" s="4"/>
+      <c r="K1004" s="4"/>
+      <c r="L1004" s="4"/>
+      <c r="M1004" s="4"/>
+      <c r="N1004" s="4"/>
+      <c r="O1004" s="4"/>
+      <c r="P1004" s="4"/>
+      <c r="Q1004" s="4"/>
+      <c r="R1004" s="4"/>
+      <c r="S1004" s="4"/>
+      <c r="T1004" s="4"/>
+      <c r="U1004" s="4"/>
+      <c r="V1004" s="4"/>
+      <c r="W1004" s="4"/>
+      <c r="X1004" s="4"/>
+      <c r="Y1004" s="4"/>
+      <c r="Z1004" s="4"/>
+    </row>
+    <row r="1005" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1005" s="6"/>
+      <c r="B1005" s="4"/>
+      <c r="C1005" s="4"/>
+      <c r="D1005" s="4"/>
+      <c r="E1005" s="4"/>
+      <c r="F1005" s="4"/>
+      <c r="G1005" s="4"/>
+      <c r="H1005" s="4"/>
+      <c r="I1005" s="4"/>
+      <c r="J1005" s="4"/>
+      <c r="K1005" s="4"/>
+      <c r="L1005" s="4"/>
+      <c r="M1005" s="4"/>
+      <c r="N1005" s="4"/>
+      <c r="O1005" s="4"/>
+      <c r="P1005" s="4"/>
+      <c r="Q1005" s="4"/>
+      <c r="R1005" s="4"/>
+      <c r="S1005" s="4"/>
+      <c r="T1005" s="4"/>
+      <c r="U1005" s="4"/>
+      <c r="V1005" s="4"/>
+      <c r="W1005" s="4"/>
+      <c r="X1005" s="4"/>
+      <c r="Y1005" s="4"/>
+      <c r="Z1005" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B13:C14"/>
-  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>